<commit_message>
fixed - edit profile and notification in register controller
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -462,7 +462,7 @@
   <dimension ref="B1:E44"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -556,7 +556,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="9" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>13</v>
@@ -571,7 +571,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
@@ -973,7 +973,7 @@
       </c>
       <c r="C44" s="18" t="n">
         <f aca="false">SUM(C6:C43)</f>
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D44" s="18" t="n">
         <v>370</v>

</xml_diff>